<commit_message>
Quick fix for direction A and D
</commit_message>
<xml_diff>
--- a/textures/angle.xlsx
+++ b/textures/angle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicagoel/Documents/cub3d/textures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6D564D-AD91-DF4F-B7B6-E8CACB7831E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59F89BF-FEFB-DF44-9CCA-0F7AACE48454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19640" yWindow="7140" windowWidth="28040" windowHeight="17440" xr2:uid="{127108D2-6415-2D47-BB31-06929C1BD9BF}"/>
+    <workbookView xWindow="5420" yWindow="5320" windowWidth="28040" windowHeight="17440" xr2:uid="{127108D2-6415-2D47-BB31-06929C1BD9BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -69,8 +69,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.0000_)_ ;_ * \(#,##0.0000\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.000000_)_ ;_ * \(#,##0.000000\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.0000_)_ ;_ * \(#,##0.0000\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.000000_)_ ;_ * \(#,##0.000000\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -127,10 +127,10 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B700F-7DAA-5340-B094-BB4BE7D9BC66}">
   <dimension ref="A2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,15 +521,15 @@
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <f>PI/$B$10*B11</f>
+        <f t="shared" ref="C11:C43" si="0">PI/$B$10*B11</f>
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <f>DISTANCE*COS(C11)</f>
+        <f t="shared" ref="E11:E43" si="1">DISTANCE*COS(C11)</f>
         <v>3</v>
       </c>
       <c r="F11" s="1">
-        <f>DISTANCE*SIN(C11)</f>
+        <f t="shared" ref="F11:F43" si="2">DISTANCE*SIN(C11)</f>
         <v>0</v>
       </c>
     </row>
@@ -538,15 +538,15 @@
         <v>1</v>
       </c>
       <c r="C12" s="2">
-        <f>PI/$B$10*B12</f>
+        <f t="shared" si="0"/>
         <v>0.19634950000000001</v>
       </c>
       <c r="E12" s="1">
-        <f>DISTANCE*COS(C12)</f>
+        <f t="shared" si="1"/>
         <v>2.9423558651176345</v>
       </c>
       <c r="F12" s="1">
-        <f>DISTANCE*SIN(C12)</f>
+        <f t="shared" si="2"/>
         <v>0.5852708458550252</v>
       </c>
     </row>
@@ -555,15 +555,15 @@
         <v>2</v>
       </c>
       <c r="C13" s="2">
-        <f>PI/$B$10*B13</f>
+        <f t="shared" si="0"/>
         <v>0.39269900000000002</v>
       </c>
       <c r="E13" s="1">
-        <f>DISTANCE*COS(C13)</f>
+        <f t="shared" si="1"/>
         <v>2.7716386913280955</v>
       </c>
       <c r="F13" s="1">
-        <f>DISTANCE*SIN(C13)</f>
+        <f t="shared" si="2"/>
         <v>1.1480500706559282</v>
       </c>
     </row>
@@ -572,15 +572,15 @@
         <v>3</v>
       </c>
       <c r="C14" s="2">
-        <f>PI/$B$10*B14</f>
+        <f t="shared" si="0"/>
         <v>0.58904850000000009</v>
       </c>
       <c r="E14" s="1">
-        <f>DISTANCE*COS(C14)</f>
+        <f t="shared" si="1"/>
         <v>2.4944090411598232</v>
       </c>
       <c r="F14" s="1">
-        <f>DISTANCE*SIN(C14)</f>
+        <f t="shared" si="2"/>
         <v>1.6667103933737653</v>
       </c>
     </row>
@@ -592,15 +592,15 @@
         <v>4</v>
       </c>
       <c r="C15" s="4">
-        <f>PI/$B$10*B15</f>
+        <f t="shared" si="0"/>
         <v>0.78539800000000004</v>
       </c>
       <c r="E15" s="1">
-        <f>DISTANCE*COS(C15)</f>
+        <f t="shared" si="1"/>
         <v>2.1213206901779453</v>
       </c>
       <c r="F15" s="1">
-        <f>DISTANCE*SIN(C15)</f>
+        <f t="shared" si="2"/>
         <v>2.121319996941283</v>
       </c>
     </row>
@@ -609,15 +609,15 @@
         <v>5</v>
       </c>
       <c r="C16" s="2">
-        <f>PI/$B$10*B16</f>
+        <f t="shared" si="0"/>
         <v>0.9817475</v>
       </c>
       <c r="E16" s="1">
-        <f>DISTANCE*COS(C16)</f>
+        <f t="shared" si="1"/>
         <v>1.6667112085338207</v>
       </c>
       <c r="F16" s="1">
-        <f>DISTANCE*SIN(C16)</f>
+        <f t="shared" si="2"/>
         <v>2.4944084964872397</v>
       </c>
     </row>
@@ -626,15 +626,15 @@
         <v>6</v>
       </c>
       <c r="C17" s="2">
-        <f>PI/$B$10*B17</f>
+        <f t="shared" si="0"/>
         <v>1.1780970000000002</v>
       </c>
       <c r="E17" s="1">
-        <f>DISTANCE*COS(C17)</f>
+        <f t="shared" si="1"/>
         <v>1.148050976413246</v>
       </c>
       <c r="F17" s="1">
-        <f>DISTANCE*SIN(C17)</f>
+        <f t="shared" si="2"/>
         <v>2.7716383161510434</v>
       </c>
     </row>
@@ -643,15 +643,15 @@
         <v>7</v>
       </c>
       <c r="C18" s="2">
-        <f>PI/$B$10*B18</f>
+        <f t="shared" si="0"/>
         <v>1.3744465000000001</v>
       </c>
       <c r="E18" s="1">
-        <f>DISTANCE*COS(C18)</f>
+        <f t="shared" si="1"/>
         <v>0.58527180740187434</v>
       </c>
       <c r="F18" s="1">
-        <f>DISTANCE*SIN(C18)</f>
+        <f t="shared" si="2"/>
         <v>2.9423556738539522</v>
       </c>
     </row>
@@ -663,15 +663,15 @@
         <v>8</v>
       </c>
       <c r="C19" s="4">
-        <f>PI/$B$10*B19</f>
+        <f t="shared" si="0"/>
         <v>1.5707960000000001</v>
       </c>
       <c r="E19" s="1">
-        <f>DISTANCE*COS(C19)</f>
+        <f t="shared" si="1"/>
         <v>9.8038468961449044E-7</v>
       </c>
       <c r="F19" s="1">
-        <f>DISTANCE*SIN(C19)</f>
+        <f t="shared" si="2"/>
         <v>2.9999999999998397</v>
       </c>
     </row>
@@ -680,15 +680,15 @@
         <v>9</v>
       </c>
       <c r="C20" s="2">
-        <f>PI/$B$10*B20</f>
+        <f t="shared" si="0"/>
         <v>1.7671455</v>
       </c>
       <c r="E20" s="1">
-        <f>DISTANCE*COS(C20)</f>
+        <f t="shared" si="1"/>
         <v>-0.58526988430811333</v>
       </c>
       <c r="F20" s="1">
-        <f>DISTANCE*SIN(C20)</f>
+        <f t="shared" si="2"/>
         <v>2.9423560563810032</v>
       </c>
     </row>
@@ -697,15 +697,15 @@
         <v>10</v>
       </c>
       <c r="C21" s="2">
-        <f>PI/$B$10*B21</f>
+        <f t="shared" si="0"/>
         <v>1.963495</v>
       </c>
       <c r="E21" s="1">
-        <f>DISTANCE*COS(C21)</f>
+        <f t="shared" si="1"/>
         <v>-1.1480491648984874</v>
       </c>
       <c r="F21" s="1">
-        <f>DISTANCE*SIN(C21)</f>
+        <f t="shared" si="2"/>
         <v>2.7716390665048518</v>
       </c>
     </row>
@@ -714,15 +714,15 @@
         <v>11</v>
       </c>
       <c r="C22" s="2">
-        <f>PI/$B$10*B22</f>
+        <f t="shared" si="0"/>
         <v>2.1598445000000002</v>
       </c>
       <c r="E22" s="1">
-        <f>DISTANCE*COS(C22)</f>
+        <f t="shared" si="1"/>
         <v>-1.6667095782135317</v>
       </c>
       <c r="F22" s="1">
-        <f>DISTANCE*SIN(C22)</f>
+        <f t="shared" si="2"/>
         <v>2.4944095858321407</v>
       </c>
     </row>
@@ -734,15 +734,15 @@
         <v>12</v>
       </c>
       <c r="C23" s="4">
-        <f>PI/$B$10*B23</f>
+        <f t="shared" si="0"/>
         <v>2.3561940000000003</v>
       </c>
       <c r="E23" s="1">
-        <f>DISTANCE*COS(C23)</f>
+        <f t="shared" si="1"/>
         <v>-2.1213193037043947</v>
       </c>
       <c r="F23" s="1">
-        <f>DISTANCE*SIN(C23)</f>
+        <f t="shared" si="2"/>
         <v>2.1213213834143803</v>
       </c>
     </row>
@@ -751,15 +751,15 @@
         <v>13</v>
       </c>
       <c r="C24" s="2">
-        <f>PI/$B$10*B24</f>
+        <f t="shared" si="0"/>
         <v>2.5525435000000001</v>
       </c>
       <c r="E24" s="1">
-        <f>DISTANCE*COS(C24)</f>
+        <f t="shared" si="1"/>
         <v>-2.4944079518143893</v>
       </c>
       <c r="F24" s="1">
-        <f>DISTANCE*SIN(C24)</f>
+        <f t="shared" si="2"/>
         <v>1.6667120236936983</v>
       </c>
     </row>
@@ -768,15 +768,15 @@
         <v>14</v>
       </c>
       <c r="C25" s="2">
-        <f>PI/$B$10*B25</f>
+        <f t="shared" si="0"/>
         <v>2.7488930000000003</v>
       </c>
       <c r="E25" s="1">
-        <f>DISTANCE*COS(C25)</f>
+        <f t="shared" si="1"/>
         <v>-2.7716379409736955</v>
       </c>
       <c r="F25" s="1">
-        <f>DISTANCE*SIN(C25)</f>
+        <f t="shared" si="2"/>
         <v>1.1480518821704415</v>
       </c>
     </row>
@@ -785,15 +785,15 @@
         <v>15</v>
       </c>
       <c r="C26" s="2">
-        <f>PI/$B$10*B26</f>
+        <f t="shared" si="0"/>
         <v>2.9452425</v>
       </c>
       <c r="E26" s="1">
-        <f>DISTANCE*COS(C26)</f>
+        <f t="shared" si="1"/>
         <v>-2.9423554825899552</v>
       </c>
       <c r="F26" s="1">
-        <f>DISTANCE*SIN(C26)</f>
+        <f t="shared" si="2"/>
         <v>0.58527276894866176</v>
       </c>
     </row>
@@ -805,15 +805,15 @@
         <v>16</v>
       </c>
       <c r="C27" s="4">
-        <f>PI/$B$10*B27</f>
+        <f t="shared" si="0"/>
         <v>3.1415920000000002</v>
       </c>
       <c r="E27" s="1">
-        <f>DISTANCE*COS(C27)</f>
+        <f t="shared" si="1"/>
         <v>-2.9999999999993592</v>
       </c>
       <c r="F27" s="1">
-        <f>DISTANCE*SIN(C27)</f>
+        <f t="shared" si="2"/>
         <v>1.9607693792288763E-6</v>
       </c>
     </row>
@@ -822,15 +822,15 @@
         <v>17</v>
       </c>
       <c r="C28" s="2">
-        <f>PI/$B$10*B28</f>
+        <f t="shared" si="0"/>
         <v>3.3379415000000003</v>
       </c>
       <c r="E28" s="1">
-        <f>DISTANCE*COS(C28)</f>
+        <f t="shared" si="1"/>
         <v>-2.942356247644057</v>
       </c>
       <c r="F28" s="1">
-        <f>DISTANCE*SIN(C28)</f>
+        <f t="shared" si="2"/>
         <v>-0.58526892276113962</v>
       </c>
     </row>
@@ -839,15 +839,15 @@
         <v>18</v>
       </c>
       <c r="C29" s="2">
-        <f>PI/$B$10*B29</f>
+        <f t="shared" si="0"/>
         <v>3.5342910000000001</v>
       </c>
       <c r="E29" s="1">
-        <f>DISTANCE*COS(C29)</f>
+        <f t="shared" si="1"/>
         <v>-2.7716394416813119</v>
       </c>
       <c r="F29" s="1">
-        <f>DISTANCE*SIN(C29)</f>
+        <f t="shared" si="2"/>
         <v>-1.148048259140924</v>
       </c>
     </row>
@@ -856,15 +856,15 @@
         <v>19</v>
       </c>
       <c r="C30" s="2">
-        <f>PI/$B$10*B30</f>
+        <f t="shared" si="0"/>
         <v>3.7306405000000002</v>
       </c>
       <c r="E30" s="1">
-        <f>DISTANCE*COS(C30)</f>
+        <f t="shared" si="1"/>
         <v>-2.4944101305041917</v>
       </c>
       <c r="F30" s="1">
-        <f>DISTANCE*SIN(C30)</f>
+        <f t="shared" si="2"/>
         <v>-1.6667087630531201</v>
       </c>
     </row>
@@ -873,15 +873,15 @@
         <v>20</v>
       </c>
       <c r="C31" s="2">
-        <f>PI/$B$10*B31</f>
+        <f t="shared" si="0"/>
         <v>3.92699</v>
       </c>
       <c r="E31" s="1">
-        <f>DISTANCE*COS(C31)</f>
+        <f t="shared" si="1"/>
         <v>-2.1213220766505905</v>
       </c>
       <c r="F31" s="1">
-        <f>DISTANCE*SIN(C31)</f>
+        <f t="shared" si="2"/>
         <v>-2.121318610467279</v>
       </c>
     </row>
@@ -890,15 +890,15 @@
         <v>21</v>
       </c>
       <c r="C32" s="2">
-        <f>PI/$B$10*B32</f>
+        <f t="shared" si="0"/>
         <v>4.1233395000000002</v>
       </c>
       <c r="E32" s="1">
-        <f>DISTANCE*COS(C32)</f>
+        <f t="shared" si="1"/>
         <v>-1.6667128388533978</v>
       </c>
       <c r="F32" s="1">
-        <f>DISTANCE*SIN(C32)</f>
+        <f t="shared" si="2"/>
         <v>-2.4944074071412725</v>
       </c>
     </row>
@@ -907,15 +907,15 @@
         <v>22</v>
       </c>
       <c r="C33" s="2">
-        <f>PI/$B$10*B33</f>
+        <f t="shared" si="0"/>
         <v>4.3196890000000003</v>
       </c>
       <c r="E33" s="1">
-        <f>DISTANCE*COS(C33)</f>
+        <f t="shared" si="1"/>
         <v>-1.1480527879275142</v>
       </c>
       <c r="F33" s="1">
-        <f>DISTANCE*SIN(C33)</f>
+        <f t="shared" si="2"/>
         <v>-2.7716375657960515</v>
       </c>
     </row>
@@ -924,15 +924,15 @@
         <v>23</v>
       </c>
       <c r="C34" s="2">
-        <f>PI/$B$10*B34</f>
+        <f t="shared" si="0"/>
         <v>4.5160385000000005</v>
       </c>
       <c r="E34" s="1">
-        <f>DISTANCE*COS(C34)</f>
+        <f t="shared" si="1"/>
         <v>-0.58527373049538478</v>
       </c>
       <c r="F34" s="1">
-        <f>DISTANCE*SIN(C34)</f>
+        <f t="shared" si="2"/>
         <v>-2.9423552913256441</v>
       </c>
     </row>
@@ -941,15 +941,15 @@
         <v>24</v>
       </c>
       <c r="C35" s="2">
-        <f>PI/$B$10*B35</f>
+        <f t="shared" si="0"/>
         <v>4.7123880000000007</v>
       </c>
       <c r="E35" s="1">
-        <f>DISTANCE*COS(C35)</f>
+        <f t="shared" si="1"/>
         <v>-2.9411540675107844E-6</v>
       </c>
       <c r="F35" s="1">
-        <f>DISTANCE*SIN(C35)</f>
+        <f t="shared" si="2"/>
         <v>-2.999999999998558</v>
       </c>
     </row>
@@ -958,15 +958,15 @@
         <v>25</v>
       </c>
       <c r="C36" s="2">
-        <f>PI/$B$10*B36</f>
+        <f t="shared" si="0"/>
         <v>4.9087375</v>
       </c>
       <c r="E36" s="1">
-        <f>DISTANCE*COS(C36)</f>
+        <f t="shared" si="1"/>
         <v>0.58526796121410163</v>
       </c>
       <c r="F36" s="1">
-        <f>DISTANCE*SIN(C36)</f>
+        <f t="shared" si="2"/>
         <v>-2.9423564389067973</v>
       </c>
     </row>
@@ -975,15 +975,15 @@
         <v>26</v>
       </c>
       <c r="C37" s="2">
-        <f>PI/$B$10*B37</f>
+        <f t="shared" si="0"/>
         <v>5.1050870000000002</v>
       </c>
       <c r="E37" s="1">
-        <f>DISTANCE*COS(C37)</f>
+        <f t="shared" si="1"/>
         <v>1.1480473533832383</v>
       </c>
       <c r="F37" s="1">
-        <f>DISTANCE*SIN(C37)</f>
+        <f t="shared" si="2"/>
         <v>-2.7716398168574758</v>
       </c>
     </row>
@@ -992,15 +992,15 @@
         <v>27</v>
       </c>
       <c r="C38" s="2">
-        <f>PI/$B$10*B38</f>
+        <f t="shared" si="0"/>
         <v>5.3014365000000003</v>
       </c>
       <c r="E38" s="1">
-        <f>DISTANCE*COS(C38)</f>
+        <f t="shared" si="1"/>
         <v>1.6667079478925304</v>
       </c>
       <c r="F38" s="1">
-        <f>DISTANCE*SIN(C38)</f>
+        <f t="shared" si="2"/>
         <v>-2.4944106751759763</v>
       </c>
     </row>
@@ -1009,15 +1009,15 @@
         <v>28</v>
       </c>
       <c r="C39" s="2">
-        <f>PI/$B$10*B39</f>
+        <f t="shared" si="0"/>
         <v>5.4977860000000005</v>
       </c>
       <c r="E39" s="1">
-        <f>DISTANCE*COS(C39)</f>
+        <f t="shared" si="1"/>
         <v>2.1213179172299377</v>
       </c>
       <c r="F39" s="1">
-        <f>DISTANCE*SIN(C39)</f>
+        <f t="shared" si="2"/>
         <v>-2.121322769886572</v>
       </c>
     </row>
@@ -1026,15 +1026,15 @@
         <v>29</v>
       </c>
       <c r="C40" s="2">
-        <f>PI/$B$10*B40</f>
+        <f t="shared" si="0"/>
         <v>5.6941355000000007</v>
       </c>
       <c r="E40" s="1">
-        <f>DISTANCE*COS(C40)</f>
+        <f t="shared" si="1"/>
         <v>2.4944068624678906</v>
       </c>
       <c r="F40" s="1">
-        <f>DISTANCE*SIN(C40)</f>
+        <f t="shared" si="2"/>
         <v>-1.6667136540129182</v>
       </c>
     </row>
@@ -1043,15 +1043,15 @@
         <v>30</v>
       </c>
       <c r="C41" s="2">
-        <f>PI/$B$10*B41</f>
+        <f t="shared" si="0"/>
         <v>5.890485</v>
       </c>
       <c r="E41" s="1">
-        <f>DISTANCE*COS(C41)</f>
+        <f t="shared" si="1"/>
         <v>2.7716371906181108</v>
       </c>
       <c r="F41" s="1">
-        <f>DISTANCE*SIN(C41)</f>
+        <f t="shared" si="2"/>
         <v>-1.1480536936844659</v>
       </c>
     </row>
@@ -1060,15 +1060,15 @@
         <v>31</v>
       </c>
       <c r="C42" s="2">
-        <f>PI/$B$10*B42</f>
+        <f t="shared" si="0"/>
         <v>6.0868345000000001</v>
       </c>
       <c r="E42" s="1">
-        <f>DISTANCE*COS(C42)</f>
+        <f t="shared" si="1"/>
         <v>2.9423551000610186</v>
       </c>
       <c r="F42" s="1">
-        <f>DISTANCE*SIN(C42)</f>
+        <f t="shared" si="2"/>
         <v>-0.58527469204204774</v>
       </c>
     </row>
@@ -1080,15 +1080,15 @@
         <v>32</v>
       </c>
       <c r="C43" s="2">
-        <f>PI/$B$10*B43</f>
+        <f t="shared" si="0"/>
         <v>6.2831840000000003</v>
       </c>
       <c r="E43" s="1">
-        <f>DISTANCE*COS(C43)</f>
+        <f t="shared" si="1"/>
         <v>2.9999999999974372</v>
       </c>
       <c r="F43" s="1">
-        <f>DISTANCE*SIN(C43)</f>
+        <f t="shared" si="2"/>
         <v>-3.9215387584569148E-6</v>
       </c>
     </row>

</xml_diff>